<commit_message>
update result data after run search
</commit_message>
<xml_diff>
--- a/Projects/2_Classical Planning/planning.xlsx
+++ b/Projects/2_Classical Planning/planning.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LinhND16\artificial-intelligence\Projects\2_Classical Planning\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Problem</t>
   </si>
@@ -123,6 +118,42 @@
   </si>
   <si>
     <t>REPORT PROJECT 2 PLANNING</t>
+  </si>
+  <si>
+    <t>Solving Air Cargo Problem 2</t>
+  </si>
+  <si>
+    <t>2.92475857123996</t>
+  </si>
+  <si>
+    <t>4.034848966198341</t>
+  </si>
+  <si>
+    <t>4.878221285477235</t>
+  </si>
+  <si>
+    <t>0.02742125020934516</t>
+  </si>
+  <si>
+    <t>5.961012654920967</t>
+  </si>
+  <si>
+    <t>11.457998789882222</t>
+  </si>
+  <si>
+    <t>25.957302062471747</t>
+  </si>
+  <si>
+    <t>3.266717609173007</t>
+  </si>
+  <si>
+    <t>185.07030858936372</t>
+  </si>
+  <si>
+    <t>1046.220499880341</t>
+  </si>
+  <si>
+    <t>3306.106357410198</t>
   </si>
 </sst>
 </file>
@@ -172,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -180,26 +211,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,7 +522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -483,357 +530,646 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
-        <v>20</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5">
         <v>43</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="5">
         <v>56</v>
       </c>
-      <c r="G3" s="3">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
         <v>178</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5">
         <v>21</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>22</v>
       </c>
-      <c r="G4" s="3">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5">
         <v>84</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="5">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5">
         <v>60</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="5">
         <v>62</v>
       </c>
-      <c r="G5" s="3">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5">
         <v>240</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="C6" s="5">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5">
         <v>7</v>
       </c>
-      <c r="E6" s="3">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="E6" s="5">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
         <v>29</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="5">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5">
         <v>6</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="5">
         <v>8</v>
       </c>
-      <c r="G7" s="3">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
         <v>28</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="5">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5">
         <v>6</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="5">
         <v>8</v>
       </c>
-      <c r="G8" s="3">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5">
         <v>24</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="C9" s="5">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5">
         <v>7</v>
       </c>
-      <c r="E9" s="3">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="E9" s="5">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
         <v>31</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="5">
+        <v>20</v>
+      </c>
+      <c r="D10" s="5">
         <v>50</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="5">
         <v>52</v>
       </c>
-      <c r="G10" s="3">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5">
         <v>206</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3">
-        <v>20</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="5">
+        <v>20</v>
+      </c>
+      <c r="D11" s="5">
         <v>28</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="5">
         <v>30</v>
       </c>
-      <c r="G11" s="3">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5">
         <v>122</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3">
-        <v>20</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="C12" s="5">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5">
         <v>43</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="5">
         <v>45</v>
       </c>
-      <c r="G12" s="3">
+      <c r="F12" s="5"/>
+      <c r="G12" s="5">
         <v>180</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="3">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="C13" s="5">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5">
         <v>51</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="5">
         <v>53</v>
       </c>
-      <c r="G13" s="3">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5">
         <v>208</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="5">
         <v>6</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5">
+        <v>72</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3343</v>
+      </c>
+      <c r="E14" s="5">
+        <v>4609</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5">
+        <v>30503</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5">
+        <v>72</v>
+      </c>
+      <c r="D15" s="5">
+        <v>624</v>
+      </c>
+      <c r="E15" s="5">
+        <v>625</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5">
+        <v>5602</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="5">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5">
+        <v>72</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5154</v>
+      </c>
+      <c r="E16" s="5">
+        <v>5156</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5">
+        <v>46618</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="5">
+        <v>72</v>
+      </c>
+      <c r="D17" s="5">
+        <v>17</v>
+      </c>
+      <c r="E17" s="5">
+        <v>19</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5">
+        <v>170</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="5">
+        <v>72</v>
+      </c>
+      <c r="D18" s="5">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5">
+        <v>11</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5">
+        <v>86</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="5">
+        <v>72</v>
+      </c>
+      <c r="D19" s="5">
+        <v>27</v>
+      </c>
+      <c r="E19" s="5">
+        <v>29</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5">
+        <v>249</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="5">
+        <v>72</v>
+      </c>
+      <c r="D20" s="5">
+        <v>26</v>
+      </c>
+      <c r="E20" s="5">
+        <v>28</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5">
+        <v>232</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="5">
+        <v>72</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2467</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2469</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5">
+        <v>22522</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="5">
+        <v>72</v>
+      </c>
+      <c r="D22" s="5">
+        <v>357</v>
+      </c>
+      <c r="E22" s="5">
+        <v>359</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5">
+        <v>3426</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="5">
+        <v>72</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2887</v>
+      </c>
+      <c r="E23" s="5">
+        <v>2889</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5">
+        <v>26594</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="5">
+        <v>72</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2102</v>
+      </c>
+      <c r="E24" s="5">
+        <v>2104</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5">
+        <v>19395</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" s="5">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:A13"/>
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A14:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF0070C0"/>
-          <x14:colorNegative rgb="FF000000"/>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FF000000"/>
-          <x14:colorFirst rgb="FF000000"/>
-          <x14:colorLast rgb="FF000000"/>
-          <x14:colorHigh rgb="FF000000"/>
-          <x14:colorLow rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B17:B17</xm:f>
-              <xm:sqref>B17</xm:sqref>
+              <xm:f>Sheet1!B28:B28</xm:f>
+              <xm:sqref>C14</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
update table result search
</commit_message>
<xml_diff>
--- a/Projects/2_Classical Planning/planning.xlsx
+++ b/Projects/2_Classical Planning/planning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Problem</t>
   </si>
@@ -154,6 +154,42 @@
   </si>
   <si>
     <t>3306.106357410198</t>
+  </si>
+  <si>
+    <t>Solving Air Cargo Problem 3</t>
+  </si>
+  <si>
+    <t>18.610267798213503</t>
+  </si>
+  <si>
+    <t>2.1803568837207052</t>
+  </si>
+  <si>
+    <t>38.62150847505466</t>
+  </si>
+  <si>
+    <t>0.0713168729324849</t>
+  </si>
+  <si>
+    <t>20.116822412587332</t>
+  </si>
+  <si>
+    <t>17.642106736679864</t>
+  </si>
+  <si>
+    <t>166.40618595028008</t>
+  </si>
+  <si>
+    <t>25.081351572574306</t>
+  </si>
+  <si>
+    <t>437.589407243675</t>
+  </si>
+  <si>
+    <t>6675.209951792273</t>
+  </si>
+  <si>
+    <t>10125.36043750458</t>
   </si>
 </sst>
 </file>
@@ -522,7 +558,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1146,11 +1182,288 @@
         <v>9</v>
       </c>
     </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="5">
+        <v>88</v>
+      </c>
+      <c r="D25" s="5">
+        <v>14663</v>
+      </c>
+      <c r="E25" s="5">
+        <v>18098</v>
+      </c>
+      <c r="G25" s="5">
+        <v>129625</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="5">
+        <v>88</v>
+      </c>
+      <c r="D26" s="5">
+        <v>408</v>
+      </c>
+      <c r="E26" s="5">
+        <v>409</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5">
+        <v>3364</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="5">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="B27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="5">
+        <v>88</v>
+      </c>
+      <c r="D27" s="5">
+        <v>18510</v>
+      </c>
+      <c r="E27" s="5">
+        <v>18512</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5">
+        <v>161936</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="5">
+        <v>88</v>
+      </c>
+      <c r="D28" s="5">
+        <v>25</v>
+      </c>
+      <c r="E28" s="5">
+        <v>27</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5">
+        <v>230</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="7"/>
+      <c r="B29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="5">
+        <v>88</v>
+      </c>
+      <c r="D29" s="5">
+        <v>14</v>
+      </c>
+      <c r="E29" s="5">
+        <v>16</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5">
+        <v>126</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="7"/>
+      <c r="B30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="5">
+        <v>88</v>
+      </c>
+      <c r="D30" s="5">
+        <v>21</v>
+      </c>
+      <c r="E30" s="5">
+        <v>23</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5">
+        <v>195</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="B31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="5">
+        <v>88</v>
+      </c>
+      <c r="D31" s="5">
+        <v>42</v>
+      </c>
+      <c r="E31" s="5">
+        <v>44</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5">
+        <v>405</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="7"/>
+      <c r="B32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="5">
+        <v>88</v>
+      </c>
+      <c r="D32" s="5">
+        <v>7388</v>
+      </c>
+      <c r="E32" s="5">
+        <v>7390</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5">
+        <v>65711</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I32" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+      <c r="B33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="5">
+        <v>88</v>
+      </c>
+      <c r="D33" s="5">
+        <v>369</v>
+      </c>
+      <c r="E33" s="5">
+        <v>371</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5">
+        <v>3403</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="7"/>
+      <c r="B34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="5">
+        <v>88</v>
+      </c>
+      <c r="D34" s="5">
+        <v>9580</v>
+      </c>
+      <c r="E34" s="5">
+        <v>9582</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5">
+        <v>86312</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="7"/>
+      <c r="B35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="5">
+        <v>88</v>
+      </c>
+      <c r="D35" s="5">
+        <v>5963</v>
+      </c>
+      <c r="E35" s="5">
+        <v>5965</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5">
+        <v>54668</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="5">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A3:A13"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A14:A24"/>
+    <mergeCell ref="A25:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1168,8 +1481,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B28:B28</xm:f>
-              <xm:sqref>C14</xm:sqref>
+              <xm:f>Sheet1!B39:B39</xm:f>
+              <xm:sqref>C25</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1189,6 +1502,22 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!B28:B28</xm:f>
+              <xm:sqref>C14</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
update new table data
</commit_message>
<xml_diff>
--- a/Projects/2_Classical Planning/planning.xlsx
+++ b/Projects/2_Classical Planning/planning.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LinhND16\artificial-intelligence\Projects\2_Classical Planning\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
   <si>
     <t>Problem</t>
   </si>
@@ -220,13 +226,25 @@
   </si>
   <si>
     <t>1046.6040979276295</t>
+  </si>
+  <si>
+    <t>P.1</t>
+  </si>
+  <si>
+    <t>P.2</t>
+  </si>
+  <si>
+    <t>P.3</t>
+  </si>
+  <si>
+    <t>P.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +272,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -269,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -292,30 +318,211 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,7 +795,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -596,1149 +803,1157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="11">
         <v>20</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="12">
         <v>43</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="11">
         <v>56</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5">
+      <c r="F3" s="11"/>
+      <c r="G3" s="12">
         <v>178</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="11">
         <v>20</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="12">
         <v>21</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="11">
         <v>22</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5">
+      <c r="F4" s="11"/>
+      <c r="G4" s="12">
         <v>84</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="14">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="11">
         <v>20</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="12">
         <v>60</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="11">
         <v>62</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5">
+      <c r="F5" s="11"/>
+      <c r="G5" s="12">
         <v>240</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="11">
         <v>20</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="12">
         <v>7</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="11">
         <v>9</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5">
+      <c r="F6" s="11"/>
+      <c r="G6" s="12">
         <v>29</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="11">
         <v>20</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="12">
         <v>6</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="11">
         <v>8</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5">
+      <c r="F7" s="11"/>
+      <c r="G7" s="12">
         <v>28</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="11">
         <v>20</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="12">
         <v>6</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="11">
         <v>8</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5">
+      <c r="F8" s="11"/>
+      <c r="G8" s="12">
         <v>24</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="11">
         <v>20</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="12">
         <v>7</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="11">
         <v>9</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5">
+      <c r="F9" s="11"/>
+      <c r="G9" s="12">
         <v>31</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="14">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="11">
         <v>20</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="12">
         <v>50</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="11">
         <v>52</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5">
+      <c r="F10" s="11"/>
+      <c r="G10" s="12">
         <v>206</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="11">
         <v>20</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="12">
         <v>28</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="11">
         <v>30</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5">
+      <c r="F11" s="11"/>
+      <c r="G11" s="12">
         <v>122</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="11">
         <v>20</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="12">
         <v>43</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="11">
         <v>45</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5">
+      <c r="F12" s="11"/>
+      <c r="G12" s="12">
         <v>180</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="11">
         <v>20</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="12">
         <v>51</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="11">
         <v>53</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5">
+      <c r="F13" s="11"/>
+      <c r="G13" s="12">
         <v>208</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="11">
         <v>72</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="12">
         <v>3343</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="11">
         <v>4609</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5">
+      <c r="F14" s="11"/>
+      <c r="G14" s="12">
         <v>30503</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="11">
         <v>72</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="12">
         <v>624</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="11">
         <v>625</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5">
+      <c r="F15" s="11"/>
+      <c r="G15" s="12">
         <v>5602</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="14">
         <v>619</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="11">
         <v>72</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="12">
         <v>5154</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="11">
         <v>5156</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5">
+      <c r="F16" s="11"/>
+      <c r="G16" s="12">
         <v>46618</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="11">
         <v>72</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="12">
         <v>17</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="11">
         <v>19</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5">
+      <c r="F17" s="11"/>
+      <c r="G17" s="12">
         <v>170</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="11">
         <v>72</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="12">
         <v>9</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="11">
         <v>11</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5">
+      <c r="F18" s="11"/>
+      <c r="G18" s="12">
         <v>86</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="11">
         <v>72</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="12">
         <v>27</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="11">
         <v>29</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5">
+      <c r="F19" s="11"/>
+      <c r="G19" s="12">
         <v>249</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="11">
         <v>72</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="12">
         <v>26</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="11">
         <v>28</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5">
+      <c r="F20" s="11"/>
+      <c r="G20" s="12">
         <v>232</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="14">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="11">
         <v>72</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="12">
         <v>2467</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="11">
         <v>2469</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5">
+      <c r="F21" s="11"/>
+      <c r="G21" s="12">
         <v>22522</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="11">
         <v>72</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="12">
         <v>357</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="11">
         <v>359</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5">
+      <c r="F22" s="11"/>
+      <c r="G22" s="12">
         <v>3426</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="11">
         <v>72</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="12">
         <v>2887</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="11">
         <v>2889</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5">
+      <c r="F23" s="11"/>
+      <c r="G23" s="12">
         <v>26594</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="5" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="11">
         <v>72</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="12">
         <v>2102</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="11">
         <v>2104</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5">
+      <c r="F24" s="11"/>
+      <c r="G24" s="12">
         <v>19395</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="11">
         <v>88</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="12">
         <v>14663</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="11">
         <v>18098</v>
       </c>
-      <c r="G25" s="5">
+      <c r="F25" s="11"/>
+      <c r="G25" s="12">
         <v>129625</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="14">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="11">
         <v>88</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="12">
         <v>408</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="11">
         <v>409</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5">
+      <c r="F26" s="11"/>
+      <c r="G26" s="12">
         <v>3364</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="14">
         <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="11">
         <v>88</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="12">
         <v>18510</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="11">
         <v>18512</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5">
+      <c r="F27" s="11"/>
+      <c r="G27" s="12">
         <v>161936</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I27" s="14">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="11">
         <v>88</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="12">
         <v>25</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="11">
         <v>27</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5">
+      <c r="F28" s="11"/>
+      <c r="G28" s="12">
         <v>230</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="14">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="11">
         <v>88</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="12">
         <v>14</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="11">
         <v>16</v>
       </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5">
+      <c r="F29" s="11"/>
+      <c r="G29" s="12">
         <v>126</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="14">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="11">
         <v>88</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="12">
         <v>21</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="11">
         <v>23</v>
       </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5">
+      <c r="F30" s="11"/>
+      <c r="G30" s="12">
         <v>195</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I30" s="14">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="11">
         <v>88</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="12">
         <v>42</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="11">
         <v>44</v>
       </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5">
+      <c r="F31" s="11"/>
+      <c r="G31" s="12">
         <v>405</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I31" s="14">
         <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="11">
         <v>88</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="12">
         <v>7388</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="11">
         <v>7390</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5">
+      <c r="F32" s="11"/>
+      <c r="G32" s="12">
         <v>65711</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I32" s="14">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="11">
         <v>88</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="12">
         <v>369</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="11">
         <v>371</v>
       </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5">
+      <c r="F33" s="11"/>
+      <c r="G33" s="12">
         <v>3403</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I33" s="14">
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="11">
         <v>88</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="12">
         <v>9580</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="11">
         <v>9582</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5">
+      <c r="F34" s="11"/>
+      <c r="G34" s="12">
         <v>86312</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="I34" s="5">
+      <c r="I34" s="14">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="11">
         <v>88</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="12">
         <v>5963</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="11">
         <v>5965</v>
       </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5">
+      <c r="F35" s="11"/>
+      <c r="G35" s="12">
         <v>54668</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H35" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I35" s="14">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="11">
         <v>104</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="12">
         <v>99736</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="11">
         <v>114953</v>
       </c>
-      <c r="G36" s="5">
+      <c r="F36" s="11"/>
+      <c r="G36" s="12">
         <v>944130</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="5">
+      <c r="I36" s="14">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="11">
         <v>104</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="12">
         <v>25174</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="11">
         <v>25175</v>
       </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5">
+      <c r="F37" s="11"/>
+      <c r="G37" s="12">
         <v>228849</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H37" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I37" s="14">
         <v>24132</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-      <c r="B38" s="4" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="11">
         <v>104</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="12">
         <v>113339</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="11">
         <v>113341</v>
       </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5">
+      <c r="F38" s="11"/>
+      <c r="G38" s="12">
         <v>1066413</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H38" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="5">
+      <c r="I38" s="14">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="4" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="11">
         <v>104</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="12">
         <v>29</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="11">
         <v>31</v>
       </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5">
+      <c r="F39" s="11"/>
+      <c r="G39" s="12">
         <v>280</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H39" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="I39" s="5">
+      <c r="I39" s="14">
         <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="5" t="s">
+      <c r="A40" s="9"/>
+      <c r="B40" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="11">
         <v>104</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="12">
         <v>17</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="11">
         <v>19</v>
       </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5">
+      <c r="F40" s="11"/>
+      <c r="G40" s="12">
         <v>165</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="H40" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I40" s="14">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="9"/>
+      <c r="B41" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="11">
         <v>104</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="12">
         <v>56</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="11">
         <v>58</v>
       </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5">
+      <c r="F41" s="11"/>
+      <c r="G41" s="12">
         <v>580</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="H41" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="5">
+      <c r="I41" s="14">
         <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="5" t="s">
+      <c r="A42" s="9"/>
+      <c r="B42" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="11">
         <v>104</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="12">
         <v>114</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="11">
         <v>116</v>
       </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5">
+      <c r="F42" s="11"/>
+      <c r="G42" s="12">
         <v>1229</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="H42" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I42" s="5">
+      <c r="I42" s="14">
         <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="5" t="s">
+      <c r="A43" s="9"/>
+      <c r="B43" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="11">
         <v>104</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="12">
         <v>34330</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="11">
         <v>34442</v>
       </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5">
+      <c r="F43" s="11"/>
+      <c r="G43" s="12">
         <v>328509</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H43" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I43" s="5">
+      <c r="I43" s="14">
         <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="5" t="s">
+      <c r="A44" s="9"/>
+      <c r="B44" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="11">
         <v>104</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="12">
         <v>1208</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="11">
         <v>1210</v>
       </c>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5">
+      <c r="F44" s="11"/>
+      <c r="G44" s="12">
         <v>12210</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="H44" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="I44" s="5">
+      <c r="I44" s="14">
         <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
-      <c r="B45" s="5" t="s">
+      <c r="A45" s="9"/>
+      <c r="B45" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="5"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="14"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="5" t="s">
+      <c r="A46" s="15"/>
+      <c r="B46" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="5"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1748,8 +1963,8 @@
     <mergeCell ref="A25:A35"/>
     <mergeCell ref="A36:A46"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.2" right="0.2" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="76" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
@@ -1764,8 +1979,24 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B50:B50</xm:f>
-              <xm:sqref>C36</xm:sqref>
+              <xm:f>Sheet1!B39:B39</xm:f>
+              <xm:sqref>C25</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!B17:B17</xm:f>
+              <xm:sqref>C3</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1796,24 +2027,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B17:B17</xm:f>
-              <xm:sqref>C3</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!B39:B39</xm:f>
-              <xm:sqref>C25</xm:sqref>
+              <xm:f>Sheet1!B50:B50</xm:f>
+              <xm:sqref>C36</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1821,4 +2036,295 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update data in new table
</commit_message>
<xml_diff>
--- a/Projects/2_Classical Planning/planning.xlsx
+++ b/Projects/2_Classical Planning/planning.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LinhND16\artificial-intelligence\Projects\2_Classical Planning\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>Problem</t>
   </si>
@@ -238,6 +233,9 @@
   </si>
   <si>
     <t>P.4</t>
+  </si>
+  <si>
+    <t>Time (seconds)</t>
   </si>
 </sst>
 </file>
@@ -457,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -481,9 +479,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
@@ -497,9 +492,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
@@ -510,11 +502,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -522,7 +521,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,7 +795,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -830,17 +830,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -872,1088 +872,1088 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>20</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>43</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <v>56</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12">
+      <c r="F3" s="10"/>
+      <c r="G3" s="11">
         <v>178</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="11">
+      <c r="A4" s="20"/>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="10">
         <v>20</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>21</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>22</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12">
+      <c r="F4" s="10"/>
+      <c r="G4" s="11">
         <v>84</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>20</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>60</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>62</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12">
+      <c r="F5" s="10"/>
+      <c r="G5" s="11">
         <v>240</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>20</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>7</v>
       </c>
-      <c r="E6" s="11">
-        <v>9</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12">
+      <c r="E6" s="10">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11">
         <v>29</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>20</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>6</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>8</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12">
+      <c r="F7" s="10"/>
+      <c r="G7" s="11">
         <v>28</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>20</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>6</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>8</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12">
+      <c r="F8" s="10"/>
+      <c r="G8" s="11">
         <v>24</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>20</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>7</v>
       </c>
-      <c r="E9" s="11">
-        <v>9</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12">
+      <c r="E9" s="10">
+        <v>9</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11">
         <v>31</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>20</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>50</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>52</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12">
+      <c r="F10" s="10"/>
+      <c r="G10" s="11">
         <v>206</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>20</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>28</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>30</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12">
+      <c r="F11" s="10"/>
+      <c r="G11" s="11">
         <v>122</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>20</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>43</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>45</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12">
+      <c r="F12" s="10"/>
+      <c r="G12" s="11">
         <v>180</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>20</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="11">
         <v>51</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>53</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12">
+      <c r="F13" s="10"/>
+      <c r="G13" s="11">
         <v>208</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>72</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>3343</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>4609</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12">
+      <c r="F14" s="10"/>
+      <c r="G14" s="11">
         <v>30503</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="11">
+      <c r="A15" s="20"/>
+      <c r="B15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="10">
         <v>72</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="11">
         <v>624</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>625</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12">
+      <c r="F15" s="10"/>
+      <c r="G15" s="11">
         <v>5602</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="13">
         <v>619</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>72</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>5154</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>5156</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12">
+      <c r="F16" s="10"/>
+      <c r="G16" s="11">
         <v>46618</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>72</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>17</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>19</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12">
+      <c r="F17" s="10"/>
+      <c r="G17" s="11">
         <v>170</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="12" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>72</v>
       </c>
-      <c r="D18" s="12">
-        <v>9</v>
-      </c>
-      <c r="E18" s="11">
+      <c r="D18" s="11">
+        <v>9</v>
+      </c>
+      <c r="E18" s="10">
         <v>11</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12">
+      <c r="F18" s="10"/>
+      <c r="G18" s="11">
         <v>86</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="20"/>
+      <c r="B19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <v>72</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="11">
         <v>27</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>29</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12">
+      <c r="F19" s="10"/>
+      <c r="G19" s="11">
         <v>249</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="12" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>72</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="11">
         <v>26</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <v>28</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="12">
+      <c r="F20" s="10"/>
+      <c r="G20" s="11">
         <v>232</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="12" t="s">
+      <c r="A21" s="20"/>
+      <c r="B21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>72</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="11">
         <v>2467</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="10">
         <v>2469</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="12">
+      <c r="F21" s="10"/>
+      <c r="G21" s="11">
         <v>22522</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="12" t="s">
+      <c r="A22" s="20"/>
+      <c r="B22" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="10">
         <v>72</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="11">
         <v>357</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="10">
         <v>359</v>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="12">
+      <c r="F22" s="10"/>
+      <c r="G22" s="11">
         <v>3426</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="20"/>
+      <c r="B23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="10">
         <v>72</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="11">
         <v>2887</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="10">
         <v>2889</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12">
+      <c r="F23" s="10"/>
+      <c r="G23" s="11">
         <v>26594</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="12" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="10">
         <v>72</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="11">
         <v>2102</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="10">
         <v>2104</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="12">
+      <c r="F24" s="10"/>
+      <c r="G24" s="11">
         <v>19395</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <v>88</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="11">
         <v>14663</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="10">
         <v>18098</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="12">
+      <c r="F25" s="10"/>
+      <c r="G25" s="11">
         <v>129625</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="H25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I25" s="13">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="11">
+      <c r="A26" s="20"/>
+      <c r="B26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="10">
         <v>88</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="11">
         <v>408</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <v>409</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="12">
+      <c r="F26" s="10"/>
+      <c r="G26" s="11">
         <v>3364</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="13">
         <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="20"/>
+      <c r="B27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="10">
         <v>88</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="11">
         <v>18510</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="10">
         <v>18512</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12">
+      <c r="F27" s="10"/>
+      <c r="G27" s="11">
         <v>161936</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="13">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10" t="s">
+      <c r="A28" s="20"/>
+      <c r="B28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="10">
         <v>88</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="11">
         <v>25</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="10">
         <v>27</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="12">
+      <c r="F28" s="10"/>
+      <c r="G28" s="11">
         <v>230</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="13">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="12" t="s">
+      <c r="A29" s="20"/>
+      <c r="B29" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="10">
         <v>88</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="11">
         <v>14</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="10">
         <v>16</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="12">
+      <c r="F29" s="10"/>
+      <c r="G29" s="11">
         <v>126</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="B30" s="12" t="s">
+      <c r="A30" s="20"/>
+      <c r="B30" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="10">
         <v>88</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="11">
         <v>21</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="10">
         <v>23</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="12">
+      <c r="F30" s="10"/>
+      <c r="G30" s="11">
         <v>195</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="13">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="B31" s="12" t="s">
+      <c r="A31" s="20"/>
+      <c r="B31" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <v>88</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="11">
         <v>42</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="10">
         <v>44</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="12">
+      <c r="F31" s="10"/>
+      <c r="G31" s="11">
         <v>405</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="13">
         <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="B32" s="12" t="s">
+      <c r="A32" s="20"/>
+      <c r="B32" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="10">
         <v>88</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <v>7388</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="10">
         <v>7390</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="12">
+      <c r="F32" s="10"/>
+      <c r="G32" s="11">
         <v>65711</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I32" s="13">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="12" t="s">
+      <c r="A33" s="20"/>
+      <c r="B33" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="10">
         <v>88</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="11">
         <v>369</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="10">
         <v>371</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="12">
+      <c r="F33" s="10"/>
+      <c r="G33" s="11">
         <v>3403</v>
       </c>
-      <c r="H33" s="13" t="s">
+      <c r="H33" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I33" s="13">
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="B34" s="12" t="s">
+      <c r="A34" s="20"/>
+      <c r="B34" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="10">
         <v>88</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="11">
         <v>9580</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="10">
         <v>9582</v>
       </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="12">
+      <c r="F34" s="10"/>
+      <c r="G34" s="11">
         <v>86312</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="I34" s="14">
+      <c r="I34" s="13">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="B35" s="12" t="s">
+      <c r="A35" s="20"/>
+      <c r="B35" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="10">
         <v>88</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="11">
         <v>5963</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="10">
         <v>5965</v>
       </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="12">
+      <c r="F35" s="10"/>
+      <c r="G35" s="11">
         <v>54668</v>
       </c>
-      <c r="H35" s="13" t="s">
+      <c r="H35" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="14">
+      <c r="I35" s="13">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="10">
         <v>104</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="11">
         <v>99736</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E36" s="10">
         <v>114953</v>
       </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="12">
+      <c r="F36" s="10"/>
+      <c r="G36" s="11">
         <v>944130</v>
       </c>
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="14">
+      <c r="I36" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="11">
+      <c r="A37" s="20"/>
+      <c r="B37" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="10">
         <v>104</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37" s="11">
         <v>25174</v>
       </c>
-      <c r="E37" s="11">
+      <c r="E37" s="10">
         <v>25175</v>
       </c>
-      <c r="F37" s="11"/>
-      <c r="G37" s="12">
+      <c r="F37" s="10"/>
+      <c r="G37" s="11">
         <v>228849</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="14">
+      <c r="I37" s="13">
         <v>24132</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
-      <c r="B38" s="10" t="s">
+      <c r="A38" s="20"/>
+      <c r="B38" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="10">
         <v>104</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38" s="11">
         <v>113339</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E38" s="10">
         <v>113341</v>
       </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="12">
+      <c r="F38" s="10"/>
+      <c r="G38" s="11">
         <v>1066413</v>
       </c>
-      <c r="H38" s="13" t="s">
+      <c r="H38" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I38" s="14">
+      <c r="I38" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="10" t="s">
+      <c r="A39" s="20"/>
+      <c r="B39" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="10">
         <v>104</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="11">
         <v>29</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E39" s="10">
         <v>31</v>
       </c>
-      <c r="F39" s="11"/>
-      <c r="G39" s="12">
+      <c r="F39" s="10"/>
+      <c r="G39" s="11">
         <v>280</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="H39" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I39" s="14">
+      <c r="I39" s="13">
         <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="12" t="s">
+      <c r="A40" s="20"/>
+      <c r="B40" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="10">
         <v>104</v>
       </c>
-      <c r="D40" s="12">
+      <c r="D40" s="11">
         <v>17</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E40" s="10">
         <v>19</v>
       </c>
-      <c r="F40" s="11"/>
-      <c r="G40" s="12">
+      <c r="F40" s="10"/>
+      <c r="G40" s="11">
         <v>165</v>
       </c>
-      <c r="H40" s="13" t="s">
+      <c r="H40" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="I40" s="14">
+      <c r="I40" s="13">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="B41" s="12" t="s">
+      <c r="A41" s="20"/>
+      <c r="B41" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="10">
         <v>104</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D41" s="11">
         <v>56</v>
       </c>
-      <c r="E41" s="11">
+      <c r="E41" s="10">
         <v>58</v>
       </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="12">
+      <c r="F41" s="10"/>
+      <c r="G41" s="11">
         <v>580</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="H41" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="I41" s="14">
+      <c r="I41" s="13">
         <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
-      <c r="B42" s="12" t="s">
+      <c r="A42" s="20"/>
+      <c r="B42" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="10">
         <v>104</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42" s="11">
         <v>114</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E42" s="10">
         <v>116</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="12">
+      <c r="F42" s="10"/>
+      <c r="G42" s="11">
         <v>1229</v>
       </c>
-      <c r="H42" s="13" t="s">
+      <c r="H42" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I42" s="14">
+      <c r="I42" s="13">
         <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="B43" s="12" t="s">
+      <c r="A43" s="20"/>
+      <c r="B43" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="10">
         <v>104</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="11">
         <v>34330</v>
       </c>
-      <c r="E43" s="11">
+      <c r="E43" s="10">
         <v>34442</v>
       </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="12">
+      <c r="F43" s="10"/>
+      <c r="G43" s="11">
         <v>328509</v>
       </c>
-      <c r="H43" s="13" t="s">
+      <c r="H43" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="I43" s="14">
+      <c r="I43" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
-      <c r="B44" s="12" t="s">
+      <c r="A44" s="20"/>
+      <c r="B44" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="10">
         <v>104</v>
       </c>
-      <c r="D44" s="12">
+      <c r="D44" s="11">
         <v>1208</v>
       </c>
-      <c r="E44" s="11">
+      <c r="E44" s="10">
         <v>1210</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="12">
+      <c r="F44" s="10"/>
+      <c r="G44" s="11">
         <v>12210</v>
       </c>
-      <c r="H44" s="13" t="s">
+      <c r="H44" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I44" s="14">
+      <c r="I44" s="13">
         <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="9"/>
-      <c r="B45" s="12" t="s">
+      <c r="A45" s="20"/>
+      <c r="B45" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="14"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="13"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
-      <c r="B46" s="16" t="s">
+      <c r="A46" s="22"/>
+      <c r="B46" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="19"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1979,8 +1979,24 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B39:B39</xm:f>
-              <xm:sqref>C25</xm:sqref>
+              <xm:f>Sheet1!B50:B50</xm:f>
+              <xm:sqref>C36</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!B28:B28</xm:f>
+              <xm:sqref>C14</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2011,24 +2027,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B28:B28</xm:f>
-              <xm:sqref>C14</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!B50:B50</xm:f>
-              <xm:sqref>C36</xm:sqref>
+              <xm:f>Sheet1!B39:B39</xm:f>
+              <xm:sqref>C25</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2042,76 +2042,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="23" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="18" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2119,203 +2123,455 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
+      <c r="B3" s="19">
+        <v>43</v>
+      </c>
+      <c r="C3" s="19">
+        <v>3343</v>
+      </c>
+      <c r="D3" s="19">
+        <v>14663</v>
+      </c>
+      <c r="E3" s="19">
+        <v>99736</v>
+      </c>
+      <c r="F3" s="26">
+        <v>8.4050470401797299E-3</v>
+      </c>
+      <c r="G3" s="19">
+        <v>2.92475857123996</v>
+      </c>
+      <c r="H3" s="19">
+        <v>18.610267798213499</v>
+      </c>
+      <c r="I3" s="19">
+        <v>94.4795746521269</v>
+      </c>
+      <c r="J3" s="19">
+        <v>6</v>
+      </c>
+      <c r="K3" s="19">
+        <v>9</v>
+      </c>
+      <c r="L3" s="19">
+        <v>12</v>
+      </c>
+      <c r="M3" s="19">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
+      <c r="B4" s="19">
+        <v>21</v>
+      </c>
+      <c r="C4" s="19">
+        <v>624</v>
+      </c>
+      <c r="D4" s="19">
+        <v>408</v>
+      </c>
+      <c r="E4" s="19">
+        <v>25174</v>
+      </c>
+      <c r="F4" s="19">
+        <v>4.0926612467945102E-3</v>
+      </c>
+      <c r="G4" s="19">
+        <v>4.0348489661983402</v>
+      </c>
+      <c r="H4" s="19">
+        <v>2.1803568837206999</v>
+      </c>
+      <c r="I4" s="19">
+        <v>3633.8678274648601</v>
+      </c>
+      <c r="J4" s="19">
+        <v>20</v>
+      </c>
+      <c r="K4" s="19">
+        <v>619</v>
+      </c>
+      <c r="L4" s="19">
+        <v>392</v>
+      </c>
+      <c r="M4" s="19">
+        <v>24132</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
+      <c r="B5" s="19">
+        <v>60</v>
+      </c>
+      <c r="C5" s="19">
+        <v>5154</v>
+      </c>
+      <c r="D5" s="19">
+        <v>18510</v>
+      </c>
+      <c r="E5" s="19">
+        <v>113339</v>
+      </c>
+      <c r="F5" s="19">
+        <v>1.17554964958366E-2</v>
+      </c>
+      <c r="G5" s="19">
+        <v>4.8782212854772302</v>
+      </c>
+      <c r="H5" s="19">
+        <v>38.621508475054597</v>
+      </c>
+      <c r="I5" s="19">
+        <v>102.603570775893</v>
+      </c>
+      <c r="J5" s="19">
+        <v>6</v>
+      </c>
+      <c r="K5" s="19">
+        <v>9</v>
+      </c>
+      <c r="L5" s="19">
+        <v>12</v>
+      </c>
+      <c r="M5" s="19">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
+      <c r="B6" s="19">
+        <v>7</v>
+      </c>
+      <c r="C6" s="19">
+        <v>17</v>
+      </c>
+      <c r="D6" s="19">
+        <v>25</v>
+      </c>
+      <c r="E6" s="19">
+        <v>29</v>
+      </c>
+      <c r="F6" s="19">
+        <v>1.96119319292421E-3</v>
+      </c>
+      <c r="G6" s="19">
+        <v>2.7421250209345101E-2</v>
+      </c>
+      <c r="H6" s="19">
+        <v>7.1316872932484898E-2</v>
+      </c>
+      <c r="I6" s="19">
+        <v>5.6899600830092802E-2</v>
+      </c>
+      <c r="J6" s="19">
+        <v>6</v>
+      </c>
+      <c r="K6" s="19">
+        <v>9</v>
+      </c>
+      <c r="L6" s="19">
+        <v>15</v>
+      </c>
+      <c r="M6" s="19">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
+      <c r="B7" s="19">
+        <v>6</v>
+      </c>
+      <c r="C7" s="19">
+        <v>9</v>
+      </c>
+      <c r="D7" s="19">
+        <v>14</v>
+      </c>
+      <c r="E7" s="19">
+        <v>17</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0.21925617409648099</v>
+      </c>
+      <c r="G7" s="19">
+        <v>5.9610126549209603</v>
+      </c>
+      <c r="H7" s="19">
+        <v>20.1168224125873</v>
+      </c>
+      <c r="I7" s="19">
+        <v>12.611480047634799</v>
+      </c>
+      <c r="J7" s="19">
+        <v>6</v>
+      </c>
+      <c r="K7" s="19">
+        <v>9</v>
+      </c>
+      <c r="L7" s="19">
+        <v>14</v>
+      </c>
+      <c r="M7" s="19">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
+      <c r="B8" s="19">
+        <v>6</v>
+      </c>
+      <c r="C8" s="19">
+        <v>27</v>
+      </c>
+      <c r="D8" s="19">
+        <v>21</v>
+      </c>
+      <c r="E8" s="19">
+        <v>56</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.15501963292472001</v>
+      </c>
+      <c r="G8" s="19">
+        <v>11.4579987898822</v>
+      </c>
+      <c r="H8" s="19">
+        <v>17.6421067366798</v>
+      </c>
+      <c r="I8" s="19">
+        <v>25.742564922485101</v>
+      </c>
+      <c r="J8" s="19">
+        <v>6</v>
+      </c>
+      <c r="K8" s="19">
+        <v>9</v>
+      </c>
+      <c r="L8" s="19">
+        <v>13</v>
+      </c>
+      <c r="M8" s="19">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
+      <c r="B9" s="19">
+        <v>7</v>
+      </c>
+      <c r="C9" s="19">
+        <v>26</v>
+      </c>
+      <c r="D9" s="19">
+        <v>42</v>
+      </c>
+      <c r="E9" s="19">
+        <v>114</v>
+      </c>
+      <c r="F9" s="19">
+        <v>0.65569350151824501</v>
+      </c>
+      <c r="G9" s="19">
+        <v>25.957302062471701</v>
+      </c>
+      <c r="H9" s="19">
+        <v>166.40618595027999</v>
+      </c>
+      <c r="I9" s="19">
+        <v>319.22763489624703</v>
+      </c>
+      <c r="J9" s="19">
+        <v>7</v>
+      </c>
+      <c r="K9" s="19">
+        <v>10</v>
+      </c>
+      <c r="L9" s="19">
+        <v>18</v>
+      </c>
+      <c r="M9" s="19">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
+      <c r="B10" s="19">
+        <v>50</v>
+      </c>
+      <c r="C10" s="19">
+        <v>2467</v>
+      </c>
+      <c r="D10" s="19">
+        <v>7388</v>
+      </c>
+      <c r="E10" s="19">
+        <v>32330</v>
+      </c>
+      <c r="F10" s="19">
+        <v>1.1974288029490601E-2</v>
+      </c>
+      <c r="G10" s="19">
+        <v>3.2667176091729999</v>
+      </c>
+      <c r="H10" s="19">
+        <v>25.081351572574299</v>
+      </c>
+      <c r="I10" s="19">
+        <v>51.813103754809099</v>
+      </c>
+      <c r="J10" s="19">
+        <v>6</v>
+      </c>
+      <c r="K10" s="19">
+        <v>9</v>
+      </c>
+      <c r="L10" s="19">
+        <v>12</v>
+      </c>
+      <c r="M10" s="19">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
+      <c r="B11" s="19">
+        <v>28</v>
+      </c>
+      <c r="C11" s="19">
+        <v>357</v>
+      </c>
+      <c r="D11" s="19">
+        <v>369</v>
+      </c>
+      <c r="E11" s="19">
+        <v>1208</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0.54208518128208105</v>
+      </c>
+      <c r="G11" s="19">
+        <v>185.07030858936301</v>
+      </c>
+      <c r="H11" s="19">
+        <v>437.589407243675</v>
+      </c>
+      <c r="I11" s="19">
+        <v>1046.6040979276199</v>
+      </c>
+      <c r="J11" s="19">
+        <v>6</v>
+      </c>
+      <c r="K11" s="19">
+        <v>9</v>
+      </c>
+      <c r="L11" s="19">
+        <v>12</v>
+      </c>
+      <c r="M11" s="19">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
+      <c r="B12" s="19">
+        <v>43</v>
+      </c>
+      <c r="C12" s="19">
+        <v>2887</v>
+      </c>
+      <c r="D12" s="19">
+        <v>9580</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19">
+        <v>0.56406416703170803</v>
+      </c>
+      <c r="G12" s="19">
+        <v>1046.22049988034</v>
+      </c>
+      <c r="H12" s="19">
+        <v>6675.2099517922697</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19">
+        <v>6</v>
+      </c>
+      <c r="K12" s="19">
+        <v>9</v>
+      </c>
+      <c r="L12" s="19">
+        <v>12</v>
+      </c>
+      <c r="M12" s="19"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
+      <c r="B13" s="19">
+        <v>51</v>
+      </c>
+      <c r="C13" s="19">
+        <v>2102</v>
+      </c>
+      <c r="D13" s="19">
+        <v>5963</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19">
+        <v>1.6050546908858101</v>
+      </c>
+      <c r="G13" s="19">
+        <v>3306.10635741019</v>
+      </c>
+      <c r="H13" s="19">
+        <v>10125.3604375045</v>
+      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19">
+        <v>6</v>
+      </c>
+      <c r="K13" s="19">
+        <v>9</v>
+      </c>
+      <c r="L13" s="19">
+        <v>12</v>
+      </c>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
update report and upload problem4.txt
</commit_message>
<xml_diff>
--- a/Projects/2_Classical Planning/planning.xlsx
+++ b/Projects/2_Classical Planning/planning.xlsx
@@ -7,9 +7,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Table analyzes" sheetId="1" r:id="rId1"/>
+    <sheet name="report" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">report!$A$1:$M$44</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="96">
   <si>
     <t>Problem</t>
   </si>
@@ -236,13 +239,250 @@
   </si>
   <si>
     <t>Time (seconds)</t>
+  </si>
+  <si>
+    <t>REPORT PROJECT 2: Classical Planing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  =&gt;  greedy_best_first_graph_search with h_unmet_goals (based on Time search)</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>Goal(At(C1, JFK) ∧ At(C2, SFO))</t>
+  </si>
+  <si>
+    <t>Goal(At(C1, JFK) ∧ At(C2, SFO) ∧ At(C3, SFO))</t>
+  </si>
+  <si>
+    <t>Goal(At(C1, JFK) ∧ At(C3, JFK) ∧ At(C2, SFO) ∧ At(C4, SFO))</t>
+  </si>
+  <si>
+    <t>Goal(At(C1, JFK) ∧ At(C2, SFO) ∧ At(C3, JFK) ∧ At(C4, SFO) ∧ At(C5, JFK))</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>P.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Solving Air Cargo Problem 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>P.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Solving Air Cargo Problem 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>P.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Solving Air Cargo Problem 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>P.4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Solving Air Cargo Problem 4</t>
+    </r>
+  </si>
+  <si>
+    <t>54027.888974003</t>
+  </si>
+  <si>
+    <t>18633.476562229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  =&gt; breadth_first_search (based on Expansions, Time and Planing length)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  =&gt; astar_search with h_unmet_goals (based on Expansions, Time)</t>
+  </si>
+  <si>
+    <t>The table analyzes the results after running the search algorithm for the problems</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Question and answer:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Which algorithm or algorithms would be most appropriate for planning problems where it is important to find only optimal plans?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Which algorithm or algorithms would be most appropriate for planning in very large domains (e.g., planning delivery routes for all UPS drivers in the U.S. on a given day)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Which algorithm or algorithms would be most appropriate for planning in a very restricted domain (i.e., one that has only a few actions) and needs to operate in real time?</t>
+    </r>
+  </si>
+  <si>
+    <t>Init(At(C1, SFO) ∧ At(C2, JFK) ∧ At(P1, SFO) ∧ At(P2, JFK) 
+      ∧ Cargo(C1) ∧ Cargo(C2) 
+      ∧ Plane(P1) ∧ Plane(P2) 
+      ∧ Airport(JFK) ∧ Airport(SFO))</t>
+  </si>
+  <si>
+    <t>Init( At(C1, SFO) ∧ At(C2, JFK) ∧ At(C3, ATL) ∧ At(P1, SFO) ∧ At(P2, JFK) ∧ At(P3, ATL) 
+       ∧ Cargo(C1) ∧ Cargo(C2) ∧ Cargo(C3)
+       ∧ Plane(P1) ∧ Plane(P2) ∧ Plane(P3)
+       ∧ Airport(JFK) ∧ Airport(SFO) ∧ Airport(ATL))</t>
+  </si>
+  <si>
+    <t>Init(At(C1, SFO) ∧ At(C2, JFK) ∧ At(C3, ATL) ∧ At(C4, ORD) ∧ At(P1, SFO) ∧ At(P2, JFK) 
+      ∧ Cargo(C1) ∧ Cargo(C2) ∧ Cargo(C3) ∧ Cargo(C4)
+      ∧ Plane(P1) ∧ Plane(P2)
+      ∧ Airport(JFK) ∧ Airport(SFO) ∧ Airport(ATL) ∧ Airport(ORD))</t>
+  </si>
+  <si>
+    <t>Init(At(C1, SFO) ∧ At(C2, JFK) ∧ At(C3, ATL) ∧ At(C4, ORD) ∧ At(C5, ORD) ∧ At(P1, SFO) ∧ At(P2, JFK)
+      ∧ Cargo(C1) ∧ Cargo(C2) ∧ Cargo(C3) ∧ Cargo(C4) ∧ Cargo(C5)
+      ∧ Plane(P1) ∧ Plane(P2)
+      ∧ Airport(JFK) ∧ Airport(SFO) ∧ Airport(ATL) ∧ Airport(ORD))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +518,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -293,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -451,11 +720,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -506,6 +784,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -515,14 +797,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,35 +1131,35 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -872,7 +1191,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -899,7 +1218,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
@@ -924,7 +1243,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
@@ -949,7 +1268,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
@@ -974,7 +1293,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
@@ -999,7 +1318,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
@@ -1024,7 +1343,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
@@ -1049,7 +1368,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
@@ -1074,7 +1393,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
@@ -1099,7 +1418,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
@@ -1124,7 +1443,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="11" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1468,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="22" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -1176,7 +1495,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="9" t="s">
         <v>9</v>
       </c>
@@ -1201,7 +1520,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="9" t="s">
         <v>10</v>
       </c>
@@ -1226,7 +1545,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
@@ -1251,7 +1570,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="11" t="s">
         <v>12</v>
       </c>
@@ -1276,7 +1595,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="11" t="s">
         <v>13</v>
       </c>
@@ -1301,7 +1620,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="11" t="s">
         <v>14</v>
       </c>
@@ -1326,7 +1645,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="11" t="s">
         <v>15</v>
       </c>
@@ -1351,7 +1670,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="11" t="s">
         <v>16</v>
       </c>
@@ -1376,7 +1695,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="11" t="s">
         <v>17</v>
       </c>
@@ -1401,7 +1720,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="11" t="s">
         <v>18</v>
       </c>
@@ -1426,7 +1745,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -1453,7 +1772,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
@@ -1478,7 +1797,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="9" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +1822,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="9" t="s">
         <v>11</v>
       </c>
@@ -1528,7 +1847,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="11" t="s">
         <v>12</v>
       </c>
@@ -1553,7 +1872,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="11" t="s">
         <v>13</v>
       </c>
@@ -1578,7 +1897,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="11" t="s">
         <v>14</v>
       </c>
@@ -1603,7 +1922,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="11" t="s">
         <v>15</v>
       </c>
@@ -1628,7 +1947,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="11" t="s">
         <v>16</v>
       </c>
@@ -1653,7 +1972,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="11" t="s">
         <v>17</v>
       </c>
@@ -1678,7 +1997,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="11" t="s">
         <v>18</v>
       </c>
@@ -1703,7 +2022,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="22" t="s">
         <v>57</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -1730,7 +2049,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="9" t="s">
         <v>9</v>
       </c>
@@ -1755,7 +2074,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="9" t="s">
         <v>10</v>
       </c>
@@ -1780,7 +2099,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="9" t="s">
         <v>11</v>
       </c>
@@ -1805,7 +2124,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="11" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +2149,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="20"/>
+      <c r="A41" s="22"/>
       <c r="B41" s="11" t="s">
         <v>13</v>
       </c>
@@ -1855,7 +2174,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="20"/>
+      <c r="A42" s="22"/>
       <c r="B42" s="11" t="s">
         <v>14</v>
       </c>
@@ -1880,7 +2199,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="20"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="11" t="s">
         <v>15</v>
       </c>
@@ -1905,7 +2224,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="11" t="s">
         <v>16</v>
       </c>
@@ -1930,30 +2249,54 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="20"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="10"/>
+      <c r="C45" s="10">
+        <v>104</v>
+      </c>
+      <c r="D45" s="11">
+        <v>62077</v>
+      </c>
+      <c r="E45" s="10">
+        <v>62079</v>
+      </c>
       <c r="F45" s="10"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="13"/>
+      <c r="G45" s="11">
+        <v>599376</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I45" s="13">
+        <v>14</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="22"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="15"/>
+      <c r="C46" s="15">
+        <v>104</v>
+      </c>
+      <c r="D46" s="14">
+        <v>37912</v>
+      </c>
+      <c r="E46" s="15">
+        <v>37914</v>
+      </c>
       <c r="F46" s="15"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="17"/>
+      <c r="G46" s="14">
+        <v>373328</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="I46" s="17">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1964,7 +2307,7 @@
     <mergeCell ref="A36:A46"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="76" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
@@ -1979,7 +2322,7 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B50:B50</xm:f>
+              <xm:f>'Table analyzes'!B50:B50</xm:f>
               <xm:sqref>C36</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
@@ -1995,7 +2338,7 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B28:B28</xm:f>
+              <xm:f>'Table analyzes'!B28:B28</xm:f>
               <xm:sqref>C14</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
@@ -2011,7 +2354,7 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B17:B17</xm:f>
+              <xm:f>'Table analyzes'!B17:B17</xm:f>
               <xm:sqref>C3</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
@@ -2027,7 +2370,7 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B39:B39</xm:f>
+              <xm:f>'Table analyzes'!B39:B39</xm:f>
               <xm:sqref>C25</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
@@ -2040,194 +2383,129 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="50.140625" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="4" width="6.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+    </row>
+    <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23" t="s">
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="18" t="s">
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C4" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D4" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G4" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H4" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I4" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K4" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L4" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M4" s="18" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="19">
-        <v>43</v>
-      </c>
-      <c r="C3" s="19">
-        <v>3343</v>
-      </c>
-      <c r="D3" s="19">
-        <v>14663</v>
-      </c>
-      <c r="E3" s="19">
-        <v>99736</v>
-      </c>
-      <c r="F3" s="26">
-        <v>8.4050470401797299E-3</v>
-      </c>
-      <c r="G3" s="19">
-        <v>2.92475857123996</v>
-      </c>
-      <c r="H3" s="19">
-        <v>18.610267798213499</v>
-      </c>
-      <c r="I3" s="19">
-        <v>94.4795746521269</v>
-      </c>
-      <c r="J3" s="19">
-        <v>6</v>
-      </c>
-      <c r="K3" s="19">
-        <v>9</v>
-      </c>
-      <c r="L3" s="19">
-        <v>12</v>
-      </c>
-      <c r="M3" s="19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="19">
-        <v>21</v>
-      </c>
-      <c r="C4" s="19">
-        <v>624</v>
-      </c>
-      <c r="D4" s="19">
-        <v>408</v>
-      </c>
-      <c r="E4" s="19">
-        <v>25174</v>
-      </c>
-      <c r="F4" s="19">
-        <v>4.0926612467945102E-3</v>
-      </c>
-      <c r="G4" s="19">
-        <v>4.0348489661983402</v>
-      </c>
-      <c r="H4" s="19">
-        <v>2.1803568837206999</v>
-      </c>
-      <c r="I4" s="19">
-        <v>3633.8678274648601</v>
-      </c>
-      <c r="J4" s="19">
-        <v>20</v>
-      </c>
-      <c r="K4" s="19">
-        <v>619</v>
-      </c>
-      <c r="L4" s="19">
-        <v>392</v>
-      </c>
-      <c r="M4" s="19">
-        <v>24132</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="19">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C5" s="19">
-        <v>5154</v>
+        <v>3343</v>
       </c>
       <c r="D5" s="19">
-        <v>18510</v>
+        <v>14663</v>
       </c>
       <c r="E5" s="19">
-        <v>113339</v>
-      </c>
-      <c r="F5" s="19">
-        <v>1.17554964958366E-2</v>
+        <v>99736</v>
+      </c>
+      <c r="F5" s="20">
+        <v>8.4050470401797299E-3</v>
       </c>
       <c r="G5" s="19">
-        <v>4.8782212854772302</v>
+        <v>2.92475857123996</v>
       </c>
       <c r="H5" s="19">
-        <v>38.621508475054597</v>
+        <v>18.610267798213499</v>
       </c>
       <c r="I5" s="19">
-        <v>102.603570775893</v>
+        <v>94.4795746521269</v>
       </c>
       <c r="J5" s="19">
         <v>6</v>
@@ -2244,72 +2522,72 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="19">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C6" s="19">
-        <v>17</v>
+        <v>624</v>
       </c>
       <c r="D6" s="19">
-        <v>25</v>
+        <v>408</v>
       </c>
       <c r="E6" s="19">
-        <v>29</v>
+        <v>25174</v>
       </c>
       <c r="F6" s="19">
-        <v>1.96119319292421E-3</v>
+        <v>4.0926612467945102E-3</v>
       </c>
       <c r="G6" s="19">
-        <v>2.7421250209345101E-2</v>
+        <v>4.0348489661983402</v>
       </c>
       <c r="H6" s="19">
-        <v>7.1316872932484898E-2</v>
+        <v>2.1803568837206999</v>
       </c>
       <c r="I6" s="19">
-        <v>5.6899600830092802E-2</v>
+        <v>3633.8678274648601</v>
       </c>
       <c r="J6" s="19">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="K6" s="19">
-        <v>9</v>
+        <v>619</v>
       </c>
       <c r="L6" s="19">
-        <v>15</v>
+        <v>392</v>
       </c>
       <c r="M6" s="19">
-        <v>18</v>
+        <v>24132</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
+      <c r="A7" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B7" s="19">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C7" s="19">
-        <v>9</v>
+        <v>5154</v>
       </c>
       <c r="D7" s="19">
-        <v>14</v>
+        <v>18510</v>
       </c>
       <c r="E7" s="19">
-        <v>17</v>
+        <v>113339</v>
       </c>
       <c r="F7" s="19">
-        <v>0.21925617409648099</v>
+        <v>1.17554964958366E-2</v>
       </c>
       <c r="G7" s="19">
-        <v>5.9610126549209603</v>
+        <v>4.8782212854772302</v>
       </c>
       <c r="H7" s="19">
-        <v>20.1168224125873</v>
+        <v>38.621508475054597</v>
       </c>
       <c r="I7" s="19">
-        <v>12.611480047634799</v>
+        <v>102.603570775893</v>
       </c>
       <c r="J7" s="19">
         <v>6</v>
@@ -2318,39 +2596,39 @@
         <v>9</v>
       </c>
       <c r="L7" s="19">
+        <v>12</v>
+      </c>
+      <c r="M7" s="19">
         <v>14</v>
       </c>
-      <c r="M7" s="19">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="19">
+        <v>7</v>
+      </c>
+      <c r="C8" s="19">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="19">
-        <v>6</v>
-      </c>
-      <c r="C8" s="19">
-        <v>27</v>
-      </c>
       <c r="D8" s="19">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E8" s="19">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="F8" s="19">
-        <v>0.15501963292472001</v>
+        <v>1.96119319292421E-3</v>
       </c>
       <c r="G8" s="19">
-        <v>11.4579987898822</v>
+        <v>2.7421250209345101E-2</v>
       </c>
       <c r="H8" s="19">
-        <v>17.6421067366798</v>
+        <v>7.1316872932484898E-2</v>
       </c>
       <c r="I8" s="19">
-        <v>25.742564922485101</v>
+        <v>5.6899600830092802E-2</v>
       </c>
       <c r="J8" s="19">
         <v>6</v>
@@ -2359,80 +2637,80 @@
         <v>9</v>
       </c>
       <c r="L8" s="19">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M8" s="19">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="19">
+        <v>6</v>
+      </c>
+      <c r="C9" s="19">
+        <v>9</v>
+      </c>
+      <c r="D9" s="19">
         <v>14</v>
       </c>
-      <c r="B9" s="19">
-        <v>7</v>
-      </c>
-      <c r="C9" s="19">
-        <v>26</v>
-      </c>
-      <c r="D9" s="19">
-        <v>42</v>
-      </c>
       <c r="E9" s="19">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="F9" s="19">
-        <v>0.65569350151824501</v>
+        <v>0.21925617409648099</v>
       </c>
       <c r="G9" s="19">
-        <v>25.957302062471701</v>
+        <v>5.9610126549209603</v>
       </c>
       <c r="H9" s="19">
-        <v>166.40618595027999</v>
+        <v>20.1168224125873</v>
       </c>
       <c r="I9" s="19">
-        <v>319.22763489624703</v>
+        <v>12.611480047634799</v>
       </c>
       <c r="J9" s="19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K9" s="19">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L9" s="19">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M9" s="19">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="19">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="C10" s="19">
-        <v>2467</v>
+        <v>27</v>
       </c>
       <c r="D10" s="19">
-        <v>7388</v>
+        <v>21</v>
       </c>
       <c r="E10" s="19">
-        <v>32330</v>
+        <v>56</v>
       </c>
       <c r="F10" s="19">
-        <v>1.1974288029490601E-2</v>
+        <v>0.15501963292472001</v>
       </c>
       <c r="G10" s="19">
-        <v>3.2667176091729999</v>
+        <v>11.4579987898822</v>
       </c>
       <c r="H10" s="19">
-        <v>25.081351572574299</v>
+        <v>17.6421067366798</v>
       </c>
       <c r="I10" s="19">
-        <v>51.813103754809099</v>
+        <v>25.742564922485101</v>
       </c>
       <c r="J10" s="19">
         <v>6</v>
@@ -2441,77 +2719,81 @@
         <v>9</v>
       </c>
       <c r="L10" s="19">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M10" s="19">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="19">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C11" s="19">
-        <v>357</v>
+        <v>26</v>
       </c>
       <c r="D11" s="19">
-        <v>369</v>
+        <v>42</v>
       </c>
       <c r="E11" s="19">
-        <v>1208</v>
+        <v>114</v>
       </c>
       <c r="F11" s="19">
-        <v>0.54208518128208105</v>
+        <v>0.65569350151824501</v>
       </c>
       <c r="G11" s="19">
-        <v>185.07030858936301</v>
+        <v>25.957302062471701</v>
       </c>
       <c r="H11" s="19">
-        <v>437.589407243675</v>
+        <v>166.40618595027999</v>
       </c>
       <c r="I11" s="19">
-        <v>1046.6040979276199</v>
+        <v>319.22763489624703</v>
       </c>
       <c r="J11" s="19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K11" s="19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L11" s="19">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="M11" s="19">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="19">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C12" s="19">
-        <v>2887</v>
+        <v>2467</v>
       </c>
       <c r="D12" s="19">
-        <v>9580</v>
-      </c>
-      <c r="E12" s="19"/>
+        <v>7388</v>
+      </c>
+      <c r="E12" s="19">
+        <v>32330</v>
+      </c>
       <c r="F12" s="19">
-        <v>0.56406416703170803</v>
+        <v>1.1974288029490601E-2</v>
       </c>
       <c r="G12" s="19">
-        <v>1046.22049988034</v>
+        <v>3.2667176091729999</v>
       </c>
       <c r="H12" s="19">
-        <v>6675.2099517922697</v>
-      </c>
-      <c r="I12" s="19"/>
+        <v>25.081351572574299</v>
+      </c>
+      <c r="I12" s="19">
+        <v>51.813103754809099</v>
+      </c>
       <c r="J12" s="19">
         <v>6</v>
       </c>
@@ -2521,32 +2803,38 @@
       <c r="L12" s="19">
         <v>12</v>
       </c>
-      <c r="M12" s="19"/>
+      <c r="M12" s="19">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="19">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C13" s="19">
-        <v>2102</v>
+        <v>357</v>
       </c>
       <c r="D13" s="19">
-        <v>5963</v>
-      </c>
-      <c r="E13" s="19"/>
+        <v>369</v>
+      </c>
+      <c r="E13" s="19">
+        <v>1208</v>
+      </c>
       <c r="F13" s="19">
-        <v>1.6050546908858101</v>
+        <v>0.54208518128208105</v>
       </c>
       <c r="G13" s="19">
-        <v>3306.10635741019</v>
+        <v>185.07030858936301</v>
       </c>
       <c r="H13" s="19">
-        <v>10125.3604375045</v>
-      </c>
-      <c r="I13" s="19"/>
+        <v>437.589407243675</v>
+      </c>
+      <c r="I13" s="19">
+        <v>1046.6040979276199</v>
+      </c>
       <c r="J13" s="19">
         <v>6</v>
       </c>
@@ -2556,31 +2844,652 @@
       <c r="L13" s="19">
         <v>12</v>
       </c>
-      <c r="M13" s="19"/>
+      <c r="M13" s="19">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="19">
+        <v>43</v>
+      </c>
+      <c r="C14" s="19">
+        <v>2887</v>
+      </c>
+      <c r="D14" s="19">
+        <v>9580</v>
+      </c>
+      <c r="E14" s="19">
+        <v>62077</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0.56406416703170803</v>
+      </c>
+      <c r="G14" s="19">
+        <v>1046.22049988034</v>
+      </c>
+      <c r="H14" s="19">
+        <v>6675.2099517922697</v>
+      </c>
+      <c r="I14" s="19">
+        <v>18633.476562229</v>
+      </c>
+      <c r="J14" s="19">
+        <v>6</v>
+      </c>
+      <c r="K14" s="19">
+        <v>9</v>
+      </c>
+      <c r="L14" s="19">
+        <v>12</v>
+      </c>
+      <c r="M14" s="19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="19">
+        <v>51</v>
+      </c>
+      <c r="C15" s="19">
+        <v>2102</v>
+      </c>
+      <c r="D15" s="19">
+        <v>5963</v>
+      </c>
+      <c r="E15" s="19">
+        <v>37912</v>
+      </c>
+      <c r="F15" s="19">
+        <v>1.6050546908858101</v>
+      </c>
+      <c r="G15" s="19">
+        <v>3306.10635741019</v>
+      </c>
+      <c r="H15" s="19">
+        <v>10125.3604375045</v>
+      </c>
+      <c r="I15" s="19">
+        <v>54027.888974002999</v>
+      </c>
+      <c r="J15" s="19">
+        <v>6</v>
+      </c>
+      <c r="K15" s="19">
+        <v>9</v>
+      </c>
+      <c r="L15" s="19">
+        <v>12</v>
+      </c>
+      <c r="M15" s="19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+    </row>
+    <row r="19" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+    </row>
+    <row r="23" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+    </row>
+    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+    </row>
+    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+    </row>
+    <row r="27" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+    </row>
+    <row r="29" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+    </row>
+    <row r="33" spans="1:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+    </row>
+    <row r="40" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
+  <mergeCells count="34">
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A19:M19"/>
+    <mergeCell ref="A21:M21"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="A30:M30"/>
+    <mergeCell ref="A22:M22"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A37:M37"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="A17:M17"/>
+    <mergeCell ref="A20:M20"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A29:M29"/>
+    <mergeCell ref="A41:M41"/>
+    <mergeCell ref="A44:M44"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A34:M34"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="A35:M35"/>
+    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="A40:M40"/>
+    <mergeCell ref="A42:M42"/>
+    <mergeCell ref="A43:M43"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.5" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="94" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>